<commit_message>
update all code to python 3
</commit_message>
<xml_diff>
--- a/data/DMSP_dosage.xlsx
+++ b/data/DMSP_dosage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtalmy/Documents/code/metro_hastings/growth_curves/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF36AD9-3544-2546-BA25-44ECDBBBEFDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F62488-2BA2-CD44-B4B5-1B4F6FC9DA7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="1900" windowWidth="28800" windowHeight="15940" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9900" yWindow="1900" windowWidth="28800" windowHeight="15940" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="379-D7 dynamics, Exp 1" sheetId="1" r:id="rId1"/>
@@ -5271,7 +5271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5250B3F-903C-9A45-8C77-FED8983B3E2D}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -5778,7 +5778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C489B84C-AF53-3F4F-BA4E-5234407B9D8B}">
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
@@ -7544,7 +7544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>

</xml_diff>